<commit_message>
Adding confusion-matrix.xlsx data and reviewing paper
</commit_message>
<xml_diff>
--- a/docs/confusion-matrix.xlsx
+++ b/docs/confusion-matrix.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\PycharmProjects\mooncake\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17BA13A-3342-44F6-AC2F-451046F16A65}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507579A7-11BC-4B21-BEA8-1A8C3E35BD27}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{EF68AD54-E154-41D6-8885-6DE605A61F1D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{EF68AD54-E154-41D6-8885-6DE605A61F1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Standard" sheetId="1" r:id="rId1"/>
+    <sheet name="ROS" sheetId="3" r:id="rId2"/>
+    <sheet name="SMOTe" sheetId="2" r:id="rId3"/>
+    <sheet name="Benchmarking" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="15">
   <si>
     <t>Non-Fraud</t>
   </si>
@@ -59,12 +62,33 @@
   <si>
     <t>SVM</t>
   </si>
+  <si>
+    <t>ROS</t>
+  </si>
+  <si>
+    <t>SMOTe</t>
+  </si>
+  <si>
+    <t>Imbalanced</t>
+  </si>
+  <si>
+    <t>Tree Classifier - validation</t>
+  </si>
+  <si>
+    <t>Random Forest - test</t>
+  </si>
+  <si>
+    <t>SVM - validation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,16 +104,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -124,11 +160,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -145,6 +196,40 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,24 +548,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6FB6925-9DCD-4DB4-93C7-7099C61C37C5}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -823,7 +904,10 @@
       <c r="L13" s="6">
         <v>979</v>
       </c>
-      <c r="N13" s="4"/>
+      <c r="N13" s="10">
+        <f>L13/SUM(K13:L13)</f>
+        <v>0.59586122945830799</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1005,4 +1089,1854 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42E2A03-C45E-42C9-A0B1-2D28CA3CE6AE}">
+  <dimension ref="A1:S27"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.140625" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5083466</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>635202</v>
+      </c>
+      <c r="F5" s="2">
+        <v>280</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>635102</v>
+      </c>
+      <c r="I5" s="2">
+        <v>357</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f>SUM(B5:C6,E5:F6,H5:I6)</f>
+        <v>11439546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5083466</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>183</v>
+      </c>
+      <c r="F6" s="6">
+        <v>597</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>239</v>
+      </c>
+      <c r="I6" s="6">
+        <v>654</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>462</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1181</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="10">
+        <f>L6/SUM(K6:L6)</f>
+        <v>0.7188070602556299</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6">
+        <f>SUM(F6,E5)/SUM(E5:F6)</f>
+        <v>0.99927231234931524</v>
+      </c>
+      <c r="S6">
+        <f>SUM(I6,H5)/SUM(H5:I6)</f>
+        <v>0.9990634114452378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="P7">
+        <f>I6/SUM(H6:I6)</f>
+        <v>0.73236282194848823</v>
+      </c>
+      <c r="S7">
+        <f>F6/SUM(E6:F6)</f>
+        <v>0.76538461538461533</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5083466</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>635109</v>
+      </c>
+      <c r="F12" s="2">
+        <v>373</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>635085</v>
+      </c>
+      <c r="I12" s="2">
+        <v>374</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f>SUM(B12:C13,E12:F13,H12:I13)</f>
+        <v>11439456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>5083466</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>165</v>
+      </c>
+      <c r="F13" s="6">
+        <v>615</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>182</v>
+      </c>
+      <c r="I13" s="6">
+        <v>621</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="6">
+        <v>422</v>
+      </c>
+      <c r="L13" s="6">
+        <v>1221</v>
+      </c>
+      <c r="N13" s="10">
+        <f>L13/SUM(K13:L13)</f>
+        <v>0.74315276932440655</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13">
+        <f>SUM(F13,E12)/SUM(E12:F13)</f>
+        <v>0.9991544363799818</v>
+      </c>
+      <c r="S13">
+        <f>SUM(I13,H12)/SUM(H12:I13)</f>
+        <v>0.99912614614734185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <f>I13/SUM(H13:I13)</f>
+        <v>0.77334993773349936</v>
+      </c>
+      <c r="S14">
+        <f>F13/SUM(E13:F13)</f>
+        <v>0.78846153846153844</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2">
+        <v>5083466</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>635422</v>
+      </c>
+      <c r="F19" s="2">
+        <v>15</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>635436</v>
+      </c>
+      <c r="I19" s="2">
+        <v>23</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <f>SUM(B19:C20,E19:F20,H19:I20)</f>
+        <v>11439456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5083466</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>216</v>
+      </c>
+      <c r="F20" s="6">
+        <v>609</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>235</v>
+      </c>
+      <c r="I20" s="6">
+        <v>568</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6">
+        <v>444</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1199</v>
+      </c>
+      <c r="N20" s="10">
+        <f>L20/SUM(K20:L20)</f>
+        <v>0.72976262933657943</v>
+      </c>
+      <c r="P20">
+        <f>SUM(F20,E19)/SUM(E19:F20)</f>
+        <v>0.99963694201445319</v>
+      </c>
+      <c r="S20">
+        <f>SUM(I20,H19)/SUM(H19:I20)</f>
+        <v>0.9995945066654931</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <f>I20/SUM(H20:I20)</f>
+        <v>0.70734744707347452</v>
+      </c>
+      <c r="S21">
+        <f>F20/SUM(E20:F20)</f>
+        <v>0.73818181818181816</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P23" s="4"/>
+    </row>
+    <row r="24" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="11"/>
+      <c r="F24" s="4"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="12"/>
+      <c r="P25" s="4"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A9:L9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D243E8-0FB9-45E7-8D97-360268BE39CF}">
+  <dimension ref="A1:S24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2">
+        <v>5083466</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>635222</v>
+      </c>
+      <c r="F5" s="2">
+        <v>260</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>635152</v>
+      </c>
+      <c r="I5" s="2">
+        <v>307</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <f>SUM(B5:C6,E5:F6,H5:I6)</f>
+        <v>11439456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5083466</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>30</v>
+      </c>
+      <c r="F6" s="6">
+        <v>750</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>41</v>
+      </c>
+      <c r="I6" s="6">
+        <v>762</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
+        <v>294</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1349</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="10">
+        <f>L6/SUM(K6:L6)</f>
+        <v>0.82105903834449179</v>
+      </c>
+      <c r="O6" s="4"/>
+      <c r="P6">
+        <f>SUM(F6,E5)/SUM(E5:F6)</f>
+        <v>0.99954421291857753</v>
+      </c>
+      <c r="S6">
+        <f>SUM(I6,H5)/SUM(H5:I6)</f>
+        <v>0.99945305550229313</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="P7">
+        <f>I6/SUM(H6:I6)</f>
+        <v>0.94894146948941471</v>
+      </c>
+      <c r="S7">
+        <f>F6/SUM(E6:F6)</f>
+        <v>0.96153846153846156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="O8" s="4"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5083466</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>635109</v>
+      </c>
+      <c r="F12" s="2">
+        <v>373</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>635085</v>
+      </c>
+      <c r="I12" s="2">
+        <v>374</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <f>SUM(B12:C13,E12:F13,H12:I13)</f>
+        <v>11439456</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6">
+        <v>5083466</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="6">
+        <v>34</v>
+      </c>
+      <c r="F13" s="6">
+        <v>746</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6">
+        <v>45</v>
+      </c>
+      <c r="I13" s="6">
+        <v>758</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="6">
+        <v>251</v>
+      </c>
+      <c r="L13" s="6">
+        <v>1392</v>
+      </c>
+      <c r="N13" s="10">
+        <f>L13/SUM(K13:L13)</f>
+        <v>0.84723067559342669</v>
+      </c>
+      <c r="O13" s="4"/>
+      <c r="P13">
+        <f>SUM(F13,E12)/SUM(E12:F13)</f>
+        <v>0.99936032640641748</v>
+      </c>
+      <c r="S13">
+        <f>SUM(I13,H12)/SUM(H12:I13)</f>
+        <v>0.99934146625132414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <f>I13/SUM(H13:I13)</f>
+        <v>0.94396014943960149</v>
+      </c>
+      <c r="S14">
+        <f>F13/SUM(E13:F13)</f>
+        <v>0.95641025641025645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="6">
+        <v>4910515</v>
+      </c>
+      <c r="C19" s="2">
+        <v>172951</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2">
+        <v>613734</v>
+      </c>
+      <c r="F19" s="2">
+        <v>21748</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="2">
+        <v>613671</v>
+      </c>
+      <c r="I19" s="2">
+        <v>21788</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <f>SUM(B19:C20,E19:F20,H19:I20)</f>
+        <v>11439456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="6">
+        <v>678349</v>
+      </c>
+      <c r="C20" s="6">
+        <v>4405117</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="6">
+        <v>103</v>
+      </c>
+      <c r="F20" s="6">
+        <v>677</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>127</v>
+      </c>
+      <c r="I20" s="6">
+        <v>676</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K20" s="6">
+        <v>273</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1370</v>
+      </c>
+      <c r="N20" s="10">
+        <f>L20/SUM(K20:L20)</f>
+        <v>0.83384053560559956</v>
+      </c>
+      <c r="P20">
+        <f>SUM(F20,E19)/SUM(E19:F20)</f>
+        <v>0.96565722925461528</v>
+      </c>
+      <c r="S20">
+        <f>SUM(I20,H19)/SUM(H19:I20)</f>
+        <v>0.96555664176078404</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="P21">
+        <f>I20/SUM(H20:I20)</f>
+        <v>0.84184308841843092</v>
+      </c>
+      <c r="S21">
+        <f>F20/SUM(E20:F20)</f>
+        <v>0.86794871794871797</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="4"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N24" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="J3:L3"/>
+    <mergeCell ref="A9:L9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31AB85E9-1AAB-4A45-B7A1-818A9B412DE4}">
+  <dimension ref="A1:R48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="11.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18" s="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" s="23"/>
+      <c r="C2" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+    </row>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B4" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B5" s="24"/>
+      <c r="C5" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="27">
+        <v>635459</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="24"/>
+      <c r="C6" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27">
+        <v>766</v>
+      </c>
+      <c r="E6" s="27">
+        <v>31</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="P7" s="13"/>
+      <c r="Q7" s="13"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="24"/>
+      <c r="C8" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="27">
+        <v>635102</v>
+      </c>
+      <c r="E8" s="27">
+        <v>357</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="24"/>
+      <c r="C9" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="27">
+        <v>239</v>
+      </c>
+      <c r="E9" s="27">
+        <v>654</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="24"/>
+      <c r="C11" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="27">
+        <v>635152</v>
+      </c>
+      <c r="E11" s="27">
+        <v>307</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="24"/>
+      <c r="C12" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="27">
+        <v>41</v>
+      </c>
+      <c r="E12" s="27">
+        <v>762</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C14" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="18"/>
+      <c r="C17" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="21">
+        <v>635437</v>
+      </c>
+      <c r="E17" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="18"/>
+      <c r="C18" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="21">
+        <v>794</v>
+      </c>
+      <c r="E18" s="21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="18"/>
+      <c r="C20" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="21">
+        <v>635202</v>
+      </c>
+      <c r="E20" s="21">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="18"/>
+      <c r="C21" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21">
+        <v>183</v>
+      </c>
+      <c r="E21" s="21">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="18"/>
+      <c r="C23" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="21">
+        <v>635222</v>
+      </c>
+      <c r="E23" s="21">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="18"/>
+      <c r="C24" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21">
+        <v>30</v>
+      </c>
+      <c r="E24" s="21">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="18"/>
+      <c r="C29" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="21">
+        <v>635459</v>
+      </c>
+      <c r="E29" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="18"/>
+      <c r="C30" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="21">
+        <v>766</v>
+      </c>
+      <c r="E30" s="21">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="18"/>
+      <c r="C32" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="21">
+        <v>635102</v>
+      </c>
+      <c r="E32" s="21">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" s="18"/>
+      <c r="C33" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="21">
+        <v>239</v>
+      </c>
+      <c r="E33" s="21">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="18"/>
+      <c r="C35" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="21">
+        <v>635152</v>
+      </c>
+      <c r="E35" s="21">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" s="18"/>
+      <c r="C36" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" s="21">
+        <v>41</v>
+      </c>
+      <c r="E36" s="21">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" s="22"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" s="22"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="22"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="22"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="22"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="22"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="22"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="19"/>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="22"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="22"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B34:B36"/>
+    <mergeCell ref="C26:E27"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C14:E15"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:E3"/>
+    <mergeCell ref="B4:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>